<commit_message>
Left optimization 1-4 done. General review
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\COBA\CODING\layerOptimizationModel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E460DE-148F-4CBC-BD44-D197787CA908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C461E913-FA93-4576-943F-01C236898795}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3977E240-FD55-4A91-9DBE-A7537FB81EA0}"/>
   </bookViews>
@@ -108,24 +108,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -459,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF06BDC8-F5BC-4487-9114-7E497B188C3E}">
-  <dimension ref="A1:R644"/>
+  <dimension ref="A1:T644"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A602" workbookViewId="0">
-      <selection activeCell="O192" sqref="O192"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -35124,7 +35114,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="593" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A593">
         <v>57775</v>
       </c>
@@ -35183,7 +35173,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="594" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A594">
         <v>57800</v>
       </c>
@@ -35242,7 +35232,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="595" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="595" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A595">
         <v>57825</v>
       </c>
@@ -35301,7 +35291,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="596" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A596">
         <v>57850</v>
       </c>
@@ -35360,7 +35350,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="597" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A597">
         <v>57875</v>
       </c>
@@ -35419,7 +35409,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="598" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="598" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A598">
         <v>57900</v>
       </c>
@@ -35478,7 +35468,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="599" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="599" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A599">
         <v>57925</v>
       </c>
@@ -35537,7 +35527,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="600" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A600">
         <v>57950</v>
       </c>
@@ -35596,7 +35586,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="601" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="601" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A601">
         <v>57975</v>
       </c>
@@ -35655,7 +35645,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="602" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A602">
         <v>58000</v>
       </c>
@@ -35714,7 +35704,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="603" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A603">
         <v>58025</v>
       </c>
@@ -35773,7 +35763,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="604" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A604">
         <v>58050</v>
       </c>
@@ -35831,8 +35821,16 @@
         <f t="shared" si="27"/>
         <v>602</v>
       </c>
-    </row>
-    <row r="605" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="S604">
+        <f>26/2</f>
+        <v>13</v>
+      </c>
+      <c r="T604">
+        <f>52/2</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="605" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A605">
         <v>58075</v>
       </c>
@@ -35891,7 +35889,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="606" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A606">
         <v>58100</v>
       </c>
@@ -35950,7 +35948,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="607" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A607">
         <v>58125</v>
       </c>
@@ -36009,7 +36007,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="608" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A608">
         <v>58150</v>
       </c>
@@ -38194,14 +38192,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="J2:O644 S192:T192 R2">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="between">
       <formula>0.001</formula>
       <formula>0.10999</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:O1048576 S192:T192 R2">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0.3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>